<commit_message>
Bug fix in rule file
</commit_message>
<xml_diff>
--- a/src/defaultrules.xlsx
+++ b/src/defaultrules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonetic-problem-generator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101FA281-AE6B-40D0-A465-A5D4F0541217}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AE9579-8083-44A7-91CC-AE8E482F6208}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18120" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
   </bookViews>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6EDC81-2F31-2B49-AF42-0AADC8A78E53}">
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
A OR logic, IMPORTANT deleted all optimization process in Rules file
All env optimizations are deleted
A OR logic implemented (may need test)
Phonme randomization is restored
</commit_message>
<xml_diff>
--- a/src/defaultrules.xlsx
+++ b/src/defaultrules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonetic-problem-generator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D3B4D6E-BAFF-4F82-9EB8-642A701B7CD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB3DED4-7774-484E-806E-D7F65EED872E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
   </bookViews>
   <sheets>
     <sheet name="defaultrules" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="194">
   <si>
     <t>&lt;&lt;PREDEFINED&gt;&gt;{'k':'t͡ʃ','g':'d͡ʒ'}/_[front,vowel]</t>
   </si>
@@ -601,6 +601,12 @@
   </si>
   <si>
     <t>[velar,fricative]&gt;[palatal,front,posterior,laminal,not strident,(secondary POA)]/_[high,front,vowel]</t>
+  </si>
+  <si>
+    <t>[consonant,voiced]&amp;[consonant,voiceless]&gt;[voiceless]/_#</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -953,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6EDC81-2F31-2B49-AF42-0AADC8A78E53}">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1978,6 +1984,17 @@
         <v>70</v>
       </c>
     </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>192</v>
+      </c>
+      <c r="B106" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tweaks on phonmes generation
</commit_message>
<xml_diff>
--- a/src/defaultrules.xlsx
+++ b/src/defaultrules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonetic-problem-generator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB3DED4-7774-484E-806E-D7F65EED872E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0995CAAD-B7DE-4856-B561-0890CFF96CBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
   </bookViews>
   <sheets>
     <sheet name="defaultrules" sheetId="1" r:id="rId1"/>
@@ -603,10 +603,10 @@
     <t>[velar,fricative]&gt;[palatal,front,posterior,laminal,not strident,(secondary POA)]/_[high,front,vowel]</t>
   </si>
   <si>
-    <t>[consonant,voiced]&amp;[consonant,voiceless]&gt;[voiceless]/_#</t>
-  </si>
-  <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>[oral stop,voiced]&amp;[affricate,voiced]&gt;[voiceless]/_#</t>
   </si>
 </sst>
 </file>
@@ -962,17 +962,17 @@
   <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="97.125" customWidth="1"/>
     <col min="2" max="2" width="72.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>117</v>
       </c>
@@ -983,7 +983,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -994,7 +994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>145</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>115</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>177</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>179</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>127</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>180</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>181</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>182</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>184</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>185</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>187</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>190</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>191</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>150</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>151</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
         <v>152</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
         <v>153</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
         <v>154</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>155</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
         <v>156</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
         <v>157</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
         <v>158</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
         <v>159</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
         <v>161</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
         <v>162</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
         <v>163</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
         <v>164</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
         <v>165</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
         <v>166</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
         <v>167</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
         <v>168</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
         <v>169</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
         <v>170</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
         <v>171</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
         <v>172</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
         <v>173</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
         <v>174</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
         <v>71</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
         <v>77</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
         <v>97</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
         <v>99</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
         <v>102</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
         <v>81</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
         <v>83</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A90" t="s">
         <v>120</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A91" t="s">
         <v>121</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A93" t="s">
         <v>113</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A94" t="s">
         <v>122</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A95" t="s">
         <v>123</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A100" t="s">
         <v>74</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A102" t="s">
         <v>124</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A103" t="s">
         <v>126</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A104" t="s">
         <v>125</v>
       </c>
@@ -1984,12 +1984,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A106" t="s">
+        <v>193</v>
+      </c>
+      <c r="B106" t="s">
         <v>192</v>
-      </c>
-      <c r="B106" t="s">
-        <v>193</v>
       </c>
       <c r="C106" t="s">
         <v>12</v>

</xml_diff>